<commit_message>
Update to Assignment 3
</commit_message>
<xml_diff>
--- a/posts/Assignment 3/DAMdatadictionary.xlsx
+++ b/posts/Assignment 3/DAMdatadictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ronald/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ronald/Desktop/U of I/PhD journey/Github/BCB521Portfolio/posts/Assignment 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC644990-1C19-994C-9BB1-A33D75C6095E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338DBD78-7323-C14A-8A43-A48E6AF67418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14500" xr2:uid="{D90452FE-51BA-5E42-B946-C16545F40E89}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Header </t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>15uM 5-HT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Serotonin diluted to 0.15uM for priming mosquitoes</t>
@@ -178,7 +175,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +493,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -526,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -534,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -542,15 +539,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -558,9 +555,7 @@
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8"/>
-      <c r="B8" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9"/>

</xml_diff>